<commit_message>
XGBoost for Cute3 done
</commit_message>
<xml_diff>
--- a/Cute3/ErrorMetrics.xlsx
+++ b/Cute3/ErrorMetrics.xlsx
@@ -48,42 +48,6 @@
     <t>LinReg_Test</t>
   </si>
   <si>
-    <t>ModelTrain</t>
-  </si>
-  <si>
-    <t>ModelTest</t>
-  </si>
-  <si>
-    <t>TrainErrorC0.001</t>
-  </si>
-  <si>
-    <t>TestErrorC0.001</t>
-  </si>
-  <si>
-    <t>TrainErrorC0.0001</t>
-  </si>
-  <si>
-    <t>TestErrorC0.0001</t>
-  </si>
-  <si>
-    <t>TrainErrorC0.0001MinSplit10</t>
-  </si>
-  <si>
-    <t>TestErrorC0.0001MinSplit10</t>
-  </si>
-  <si>
-    <t>TrainErrorC0.0001MinSplit50</t>
-  </si>
-  <si>
-    <t>TestErrorC0.0001MinSplit50</t>
-  </si>
-  <si>
-    <t>TrainErrorC0.0002MinSplit10</t>
-  </si>
-  <si>
-    <t>TestErrorC0.0002MinSplit10</t>
-  </si>
-  <si>
     <t>mae</t>
   </si>
   <si>
@@ -94,6 +58,42 @@
   </si>
   <si>
     <t>mape</t>
+  </si>
+  <si>
+    <t>TrainCP0.01</t>
+  </si>
+  <si>
+    <t>TestCP0.01</t>
+  </si>
+  <si>
+    <t>TrainCP0.001</t>
+  </si>
+  <si>
+    <t>TestCP0.001</t>
+  </si>
+  <si>
+    <t>TrainCP0.0001</t>
+  </si>
+  <si>
+    <t>TestCP0.0001</t>
+  </si>
+  <si>
+    <t>TrainCP0.0001_MinSp10</t>
+  </si>
+  <si>
+    <t>TrainCP0.0001_MinSp10.1</t>
+  </si>
+  <si>
+    <t>Train0.00001_MinSp10</t>
+  </si>
+  <si>
+    <t>Test0.00001_MinSp10</t>
+  </si>
+  <si>
+    <t>Train0.00002_MinSp10</t>
+  </si>
+  <si>
+    <t>Test0.00002_MinSp10</t>
   </si>
 </sst>
 </file>
@@ -109,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,14 +135,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -414,7 +449,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +529,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,204 +539,204 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>15.702858614078499</v>
+        <v>1.05569027399669</v>
       </c>
       <c r="C2">
-        <v>15.494580459224499</v>
+        <v>1.05190514749282</v>
       </c>
       <c r="D2">
-        <v>12.2223844120889</v>
+        <v>0.81217515351616598</v>
       </c>
       <c r="E2">
-        <v>12.463934338404901</v>
-      </c>
-      <c r="F2">
-        <v>10.0844643550728</v>
-      </c>
-      <c r="G2">
-        <v>10.578630431358899</v>
+        <v>0.80809969373582002</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.68989815808176602</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.70770995155222904</v>
       </c>
       <c r="H2">
-        <v>9.8231432924130893</v>
+        <v>0.68552576753924599</v>
       </c>
       <c r="I2">
-        <v>10.641698352669099</v>
+        <v>0.71067366279937405</v>
       </c>
       <c r="J2">
-        <v>10.435269936405099</v>
+        <v>0.454464456272199</v>
       </c>
       <c r="K2">
-        <v>10.683262336595</v>
+        <v>0.80405455103368895</v>
       </c>
       <c r="L2">
-        <v>10.9765424500024</v>
+        <v>0.72946724337832602</v>
       </c>
       <c r="M2">
-        <v>11.386450572489901</v>
+        <v>0.73368388849503097</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>611.847319121027</v>
+        <v>1.91940610862456</v>
       </c>
       <c r="C3">
-        <v>639.68258347899598</v>
+        <v>1.8989350078844101</v>
       </c>
       <c r="D3">
-        <v>362.63322990023499</v>
+        <v>1.2200367332072899</v>
       </c>
       <c r="E3">
-        <v>421.24088232105498</v>
-      </c>
-      <c r="F3">
-        <v>252.34778673786499</v>
-      </c>
-      <c r="G3">
-        <v>338.20062003735802</v>
+        <v>1.2303173328936401</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.92771673787272002</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.02770054103641</v>
       </c>
       <c r="H3">
-        <v>229.108769131462</v>
+        <v>0.90739142363824299</v>
       </c>
       <c r="I3">
-        <v>343.57956865448</v>
+        <v>1.0400438064044799</v>
       </c>
       <c r="J3">
-        <v>304.49054036062603</v>
+        <v>0.42847650866287101</v>
       </c>
       <c r="K3">
-        <v>344.48860840241798</v>
+        <v>1.3991635617348801</v>
       </c>
       <c r="L3">
-        <v>285.76437981857998</v>
+        <v>1.01868441349299</v>
       </c>
       <c r="M3">
-        <v>360.57499065826198</v>
+        <v>1.0692727891987499</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>24.735547681848999</v>
+        <v>1.38542632738972</v>
       </c>
       <c r="C4">
-        <v>25.291947008464899</v>
+        <v>1.37801850781635</v>
       </c>
       <c r="D4">
-        <v>19.042931231830799</v>
+        <v>1.10455272993519</v>
       </c>
       <c r="E4">
-        <v>20.524153632270799</v>
-      </c>
-      <c r="F4">
-        <v>15.885458342077101</v>
-      </c>
-      <c r="G4">
-        <v>18.390231647191399</v>
+        <v>1.1091967061318</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.96318053233686196</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.01375566140782</v>
       </c>
       <c r="H4">
-        <v>15.1363393570395</v>
+        <v>0.952570954647602</v>
       </c>
       <c r="I4">
-        <v>18.535899456311299</v>
+        <v>1.0198253803492501</v>
       </c>
       <c r="J4">
-        <v>17.4496573135585</v>
+        <v>0.65458117041576402</v>
       </c>
       <c r="K4">
-        <v>18.560404316782002</v>
+        <v>1.1828624441307101</v>
       </c>
       <c r="L4">
-        <v>16.904566833213401</v>
+        <v>1.00929897131276</v>
       </c>
       <c r="M4">
-        <v>18.988812249802798</v>
+        <v>1.0340564729253201</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>8.3769597863504508</v>
+        <v>0.31414610963362999</v>
       </c>
       <c r="C5">
-        <v>9.0488253263975906</v>
+        <v>0.31886647906499699</v>
       </c>
       <c r="D5">
-        <v>5.5710544091160603</v>
+        <v>0.247710487123041</v>
       </c>
       <c r="E5">
-        <v>6.0194473764400698</v>
-      </c>
-      <c r="F5">
-        <v>3.9027376588495901</v>
-      </c>
-      <c r="G5">
-        <v>4.12969363158488</v>
+        <v>0.24863476468752399</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.188502275545435</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.18948469970419701</v>
       </c>
       <c r="H5">
-        <v>3.9010139557005901</v>
+        <v>0.188092578765611</v>
       </c>
       <c r="I5">
-        <v>4.1299905517639699</v>
+        <v>0.189911559401402</v>
       </c>
       <c r="J5">
-        <v>3.9043412570659699</v>
+        <v>0.118854461751733</v>
       </c>
       <c r="K5">
-        <v>4.1298120707767803</v>
+        <v>0.209367742733573</v>
       </c>
       <c r="L5">
-        <v>4.1010114885737003</v>
+        <v>0.19473742295281701</v>
       </c>
       <c r="M5">
-        <v>4.3363334684619703</v>
+        <v>0.19392897955701499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>